<commit_message>
fim run: redo 05-2024 run with original supply side IRA numbers to check work
</commit_message>
<xml_diff>
--- a/results/05-2024/comparison-deflators-05-2024.xlsx
+++ b/results/05-2024/comparison-deflators-05-2024.xlsx
@@ -883,52 +883,52 @@
         <v>-0.0708</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0969</v>
+        <v>0.1067</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.045</v>
+        <v>-0.0452</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2751</v>
+        <v>0.295</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2384</v>
+        <v>0.2573</v>
       </c>
       <c r="L6" t="n">
-        <v>0.5026</v>
+        <v>0.3088</v>
       </c>
       <c r="M6" t="n">
-        <v>0.5367</v>
+        <v>0.2796</v>
       </c>
       <c r="N6" t="n">
-        <v>0.7111</v>
+        <v>0.1561</v>
       </c>
       <c r="O6" t="n">
-        <v>0.3556</v>
+        <v>-0.1221</v>
       </c>
       <c r="P6" t="n">
-        <v>0.1834</v>
+        <v>-0.2406</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.1366</v>
+        <v>-0.226</v>
       </c>
       <c r="R6" t="n">
-        <v>0.0037</v>
+        <v>-0.2871</v>
       </c>
       <c r="S6" t="n">
-        <v>0.0363</v>
+        <v>-0.2221</v>
       </c>
       <c r="T6" t="n">
-        <v>0.0316</v>
+        <v>-0.1724</v>
       </c>
       <c r="U6" t="n">
-        <v>0.0962</v>
+        <v>-0.035</v>
       </c>
       <c r="V6" t="n">
-        <v>0.122</v>
+        <v>-0.1145</v>
       </c>
       <c r="W6" t="n">
-        <v>-3.7756</v>
+        <v>-0.4321</v>
       </c>
     </row>
     <row r="7">
@@ -1593,52 +1593,52 @@
         <v>-4.5905</v>
       </c>
       <c r="H16" t="n">
-        <v>-2.2972</v>
+        <v>-2.2874</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.5605</v>
+        <v>-0.5607</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0439</v>
+        <v>0.0638</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.2074</v>
+        <v>-0.1884</v>
       </c>
       <c r="L16" t="n">
-        <v>0.7225</v>
+        <v>0.5287</v>
       </c>
       <c r="M16" t="n">
-        <v>0.4883</v>
+        <v>0.2312</v>
       </c>
       <c r="N16" t="n">
-        <v>0.3005</v>
+        <v>-0.2545</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.2837</v>
+        <v>-0.7614</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.0332</v>
+        <v>-0.4572</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.1419</v>
+        <v>-0.2208</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.5106</v>
+        <v>-0.8013</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.6713</v>
+        <v>-0.9297</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.4579</v>
+        <v>-0.6619</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.3235</v>
+        <v>-0.4547</v>
       </c>
       <c r="V16" t="n">
-        <v>0.0767</v>
+        <v>-0.1598</v>
       </c>
       <c r="W16" t="n">
-        <v>-75.1223</v>
+        <v>-71.7788</v>
       </c>
     </row>
     <row r="17">
@@ -2871,52 +2871,52 @@
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>-0.0098</v>
+        <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>0.0002</v>
+        <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>-0.0199</v>
+        <v>0</v>
       </c>
       <c r="K34" t="n">
-        <v>-0.019</v>
+        <v>0</v>
       </c>
       <c r="L34" t="n">
-        <v>0.1938</v>
+        <v>0</v>
       </c>
       <c r="M34" t="n">
-        <v>0.2571</v>
+        <v>0</v>
       </c>
       <c r="N34" t="n">
-        <v>0.555</v>
+        <v>0</v>
       </c>
       <c r="O34" t="n">
-        <v>0.4759</v>
+        <v>-0.0018</v>
       </c>
       <c r="P34" t="n">
-        <v>0.4215</v>
+        <v>-0.0024</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.3602</v>
+        <v>-0.0025</v>
       </c>
       <c r="R34" t="n">
-        <v>0.2876</v>
+        <v>-0.0032</v>
       </c>
       <c r="S34" t="n">
-        <v>0.2558</v>
+        <v>-0.0026</v>
       </c>
       <c r="T34" t="n">
-        <v>0.2023</v>
+        <v>-0.0017</v>
       </c>
       <c r="U34" t="n">
-        <v>0.1317</v>
+        <v>0.0005</v>
       </c>
       <c r="V34" t="n">
-        <v>0.2361</v>
+        <v>-0.0004</v>
       </c>
       <c r="W34" t="n">
-        <v>-3.3484</v>
+        <v>-0.0049</v>
       </c>
     </row>
     <row r="35">
@@ -3581,52 +3581,52 @@
         <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>-0.0098</v>
+        <v>0</v>
       </c>
       <c r="I44" t="n">
-        <v>0.0002</v>
+        <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>-0.0199</v>
+        <v>0</v>
       </c>
       <c r="K44" t="n">
-        <v>-0.019</v>
+        <v>0</v>
       </c>
       <c r="L44" t="n">
-        <v>0.1938</v>
+        <v>0</v>
       </c>
       <c r="M44" t="n">
-        <v>0.2571</v>
+        <v>0</v>
       </c>
       <c r="N44" t="n">
-        <v>0.555</v>
+        <v>0</v>
       </c>
       <c r="O44" t="n">
-        <v>0.3901</v>
+        <v>-0.0876</v>
       </c>
       <c r="P44" t="n">
-        <v>0.3298</v>
+        <v>-0.0942</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.2609</v>
+        <v>-0.1018</v>
       </c>
       <c r="R44" t="n">
-        <v>0.1757</v>
+        <v>-0.1151</v>
       </c>
       <c r="S44" t="n">
-        <v>0.1482</v>
+        <v>-0.1102</v>
       </c>
       <c r="T44" t="n">
-        <v>0.1063</v>
+        <v>-0.0977</v>
       </c>
       <c r="U44" t="n">
-        <v>0.0469</v>
+        <v>-0.0843</v>
       </c>
       <c r="V44" t="n">
-        <v>0.1676</v>
+        <v>-0.0689</v>
       </c>
       <c r="W44" t="n">
-        <v>-4.4752</v>
+        <v>-1.1317</v>
       </c>
     </row>
     <row r="45">

</xml_diff>

<commit_message>
run: use new supply side/IRA assumptions
</commit_message>
<xml_diff>
--- a/results/05-2024/comparison-deflators-05-2024.xlsx
+++ b/results/05-2024/comparison-deflators-05-2024.xlsx
@@ -883,52 +883,52 @@
         <v>-0.0708</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1067</v>
+        <v>0.0969</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.0452</v>
+        <v>-0.045</v>
       </c>
       <c r="J6" t="n">
-        <v>0.295</v>
+        <v>0.2751</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2573</v>
+        <v>0.2384</v>
       </c>
       <c r="L6" t="n">
-        <v>0.3088</v>
+        <v>0.5026</v>
       </c>
       <c r="M6" t="n">
-        <v>0.2796</v>
+        <v>0.0985</v>
       </c>
       <c r="N6" t="n">
-        <v>0.1561</v>
+        <v>0.087</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.1221</v>
+        <v>0.0027</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.2406</v>
+        <v>-0.0924</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.226</v>
+        <v>-0.0876</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.2871</v>
+        <v>-0.1505</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.2221</v>
+        <v>-0.0734</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.1724</v>
+        <v>-0.0804</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.035</v>
+        <v>-0.0891</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.1145</v>
+        <v>-0.0788</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.4321</v>
+        <v>-1.0948</v>
       </c>
     </row>
     <row r="7">
@@ -1593,52 +1593,52 @@
         <v>-4.5905</v>
       </c>
       <c r="H16" t="n">
-        <v>-2.2874</v>
+        <v>-2.2972</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.5607</v>
+        <v>-0.5605</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0638</v>
+        <v>0.0439</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.1884</v>
+        <v>-0.2074</v>
       </c>
       <c r="L16" t="n">
-        <v>0.5287</v>
+        <v>0.7225</v>
       </c>
       <c r="M16" t="n">
-        <v>0.2312</v>
+        <v>0.0501</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.2545</v>
+        <v>-0.3236</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.7614</v>
+        <v>-0.6367</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.4572</v>
+        <v>-0.309</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.2208</v>
+        <v>-0.0824</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.8013</v>
+        <v>-0.6647</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.9297</v>
+        <v>-0.7811</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.6619</v>
+        <v>-0.5699</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.4547</v>
+        <v>-0.5089</v>
       </c>
       <c r="V16" t="n">
-        <v>-0.1598</v>
+        <v>-0.124</v>
       </c>
       <c r="W16" t="n">
-        <v>-71.7788</v>
+        <v>-72.4415</v>
       </c>
     </row>
     <row r="17">
@@ -2871,52 +2871,52 @@
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>0</v>
+        <v>-0.0098</v>
       </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="J34" t="n">
-        <v>0</v>
+        <v>-0.0199</v>
       </c>
       <c r="K34" t="n">
-        <v>0</v>
+        <v>-0.019</v>
       </c>
       <c r="L34" t="n">
-        <v>0</v>
+        <v>0.1938</v>
       </c>
       <c r="M34" t="n">
-        <v>0</v>
+        <v>-0.1811</v>
       </c>
       <c r="N34" t="n">
-        <v>0</v>
+        <v>-0.0691</v>
       </c>
       <c r="O34" t="n">
-        <v>-0.0018</v>
+        <v>0.1229</v>
       </c>
       <c r="P34" t="n">
-        <v>-0.0024</v>
+        <v>0.1457</v>
       </c>
       <c r="Q34" t="n">
-        <v>-0.0025</v>
+        <v>0.1359</v>
       </c>
       <c r="R34" t="n">
-        <v>-0.0032</v>
+        <v>0.1334</v>
       </c>
       <c r="S34" t="n">
-        <v>-0.0026</v>
+        <v>0.146</v>
       </c>
       <c r="T34" t="n">
-        <v>-0.0017</v>
+        <v>0.0903</v>
       </c>
       <c r="U34" t="n">
-        <v>0.0005</v>
+        <v>-0.0537</v>
       </c>
       <c r="V34" t="n">
-        <v>-0.0004</v>
+        <v>0.0354</v>
       </c>
       <c r="W34" t="n">
-        <v>-0.0049</v>
+        <v>-0.6676</v>
       </c>
     </row>
     <row r="35">
@@ -3581,52 +3581,52 @@
         <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>0</v>
+        <v>-0.0098</v>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="J44" t="n">
-        <v>0</v>
+        <v>-0.0199</v>
       </c>
       <c r="K44" t="n">
-        <v>0</v>
+        <v>-0.019</v>
       </c>
       <c r="L44" t="n">
-        <v>0</v>
+        <v>0.1938</v>
       </c>
       <c r="M44" t="n">
-        <v>0</v>
+        <v>-0.1811</v>
       </c>
       <c r="N44" t="n">
-        <v>0</v>
+        <v>-0.0691</v>
       </c>
       <c r="O44" t="n">
-        <v>-0.0876</v>
+        <v>0.0371</v>
       </c>
       <c r="P44" t="n">
-        <v>-0.0942</v>
+        <v>0.054</v>
       </c>
       <c r="Q44" t="n">
-        <v>-0.1018</v>
+        <v>0.0367</v>
       </c>
       <c r="R44" t="n">
-        <v>-0.1151</v>
+        <v>0.0215</v>
       </c>
       <c r="S44" t="n">
-        <v>-0.1102</v>
+        <v>0.0384</v>
       </c>
       <c r="T44" t="n">
-        <v>-0.0977</v>
+        <v>-0.0057</v>
       </c>
       <c r="U44" t="n">
-        <v>-0.0843</v>
+        <v>-0.1384</v>
       </c>
       <c r="V44" t="n">
-        <v>-0.0689</v>
+        <v>-0.0331</v>
       </c>
       <c r="W44" t="n">
-        <v>-1.1317</v>
+        <v>-1.7944</v>
       </c>
     </row>
     <row r="45">

</xml_diff>

<commit_message>
run: with new 2026 Q1 forecast + Haver pull, without MPI
</commit_message>
<xml_diff>
--- a/results/05-2024/comparison-deflators-05-2024.xlsx
+++ b/results/05-2024/comparison-deflators-05-2024.xlsx
@@ -617,7 +617,7 @@
         <v>0.0044</v>
       </c>
       <c r="N2" t="n">
-        <v>0.0084</v>
+        <v>0.0082</v>
       </c>
       <c r="O2" t="n">
         <v>0.0067</v>
@@ -641,7 +641,7 @@
         <v>0.0053</v>
       </c>
       <c r="V2" t="n">
-        <v>0</v>
+        <v>0.0053</v>
       </c>
       <c r="W2" t="n">
         <v>0.0051</v>
@@ -691,31 +691,31 @@
         <v>310.9897</v>
       </c>
       <c r="O3" t="n">
-        <v>311.58</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>313.653</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>315.562</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>317.539</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>319.487</v>
+        <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>321.422</v>
+        <v>0</v>
       </c>
       <c r="U3" t="n">
-        <v>323.328</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>325.189</v>
+        <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>327.004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -765,7 +765,7 @@
         <v>-0.0177</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.0671</v>
+        <v>-0.0672</v>
       </c>
       <c r="Q4" t="n">
         <v>-0.0292</v>
@@ -774,7 +774,7 @@
         <v>-0.0283</v>
       </c>
       <c r="S4" t="n">
-        <v>-0.0267</v>
+        <v>-0.0268</v>
       </c>
       <c r="T4" t="n">
         <v>-0.026</v>
@@ -830,34 +830,34 @@
         <v>0.1538</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.2668</v>
+        <v>-0.3011</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.3996</v>
+        <v>-0.3991</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.1087</v>
+        <v>-0.1106</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.1253</v>
+        <v>-0.1223</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.4667</v>
+        <v>-0.4687</v>
       </c>
       <c r="S5" t="n">
-        <v>-0.3414</v>
+        <v>-0.3419</v>
       </c>
       <c r="T5" t="n">
-        <v>-0.1712</v>
+        <v>-0.1742</v>
       </c>
       <c r="U5" t="n">
-        <v>-0.2057</v>
+        <v>-0.2067</v>
       </c>
       <c r="V5" t="n">
-        <v>-0.1419</v>
+        <v>-0.1357</v>
       </c>
       <c r="W5" t="n">
-        <v>-31.9196</v>
+        <v>-32.136</v>
       </c>
     </row>
     <row r="6">
@@ -901,34 +901,34 @@
         <v>0.2796</v>
       </c>
       <c r="N6" t="n">
-        <v>0.1561</v>
+        <v>0.1478</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.1221</v>
+        <v>-0.023</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.2406</v>
+        <v>-0.0289</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.226</v>
+        <v>-0.0223</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.2871</v>
+        <v>-0.0168</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.2221</v>
+        <v>0.0041</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.1724</v>
+        <v>-0.0039</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.035</v>
+        <v>-0.0134</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.1145</v>
+        <v>-0.0281</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.4321</v>
+        <v>-1.794</v>
       </c>
     </row>
     <row r="7">
@@ -972,34 +972,34 @@
         <v>-0.1622</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.2224</v>
+        <v>-0.2068</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.1893</v>
+        <v>-0.167</v>
       </c>
       <c r="P7" t="n">
-        <v>0.0271</v>
+        <v>0.0162</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.0196</v>
+        <v>-0.0276</v>
       </c>
       <c r="R7" t="n">
-        <v>0.031</v>
+        <v>0.0109</v>
       </c>
       <c r="S7" t="n">
-        <v>0.0205</v>
+        <v>-0.0032</v>
       </c>
       <c r="T7" t="n">
-        <v>0.0081</v>
+        <v>0.0192</v>
       </c>
       <c r="U7" t="n">
-        <v>0.0252</v>
+        <v>0.0327</v>
       </c>
       <c r="V7" t="n">
-        <v>0.0701</v>
+        <v>0.0471</v>
       </c>
       <c r="W7" t="n">
-        <v>-5.1218</v>
+        <v>-5.1508</v>
       </c>
     </row>
     <row r="8">
@@ -1040,37 +1040,37 @@
         <v>0.3669</v>
       </c>
       <c r="M8" t="n">
-        <v>0.3659</v>
+        <v>0.4046</v>
       </c>
       <c r="N8" t="n">
-        <v>0.2014</v>
+        <v>0.303</v>
       </c>
       <c r="O8" t="n">
-        <v>0.119</v>
+        <v>0.2001</v>
       </c>
       <c r="P8" t="n">
-        <v>0.2924</v>
+        <v>0.3412</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.2333</v>
+        <v>0.2815</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.1073</v>
+        <v>-0.0589</v>
       </c>
       <c r="S8" t="n">
-        <v>-0.1214</v>
+        <v>-0.0737</v>
       </c>
       <c r="T8" t="n">
-        <v>-0.0895</v>
+        <v>-0.0432</v>
       </c>
       <c r="U8" t="n">
-        <v>-0.0792</v>
+        <v>-0.0514</v>
       </c>
       <c r="V8" t="n">
-        <v>-0.0253</v>
+        <v>0.0313</v>
       </c>
       <c r="W8" t="n">
-        <v>7.6169</v>
+        <v>7.5608</v>
       </c>
     </row>
     <row r="9">
@@ -1117,10 +1117,10 @@
         <v>-0.0373</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.0357</v>
+        <v>-0.0358</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.0345</v>
+        <v>-0.0346</v>
       </c>
       <c r="Q9" t="n">
         <v>-0.0226</v>
@@ -1212,7 +1212,7 @@
         <v>-0.007</v>
       </c>
       <c r="W10" t="n">
-        <v>-0.0064</v>
+        <v>-0.0065</v>
       </c>
     </row>
     <row r="11">
@@ -1256,7 +1256,7 @@
         <v>0.0098</v>
       </c>
       <c r="N11" t="n">
-        <v>0.0101</v>
+        <v>0.0112</v>
       </c>
       <c r="O11" t="n">
         <v>0.0078</v>
@@ -1280,7 +1280,7 @@
         <v>0.0061</v>
       </c>
       <c r="V11" t="n">
-        <v>0</v>
+        <v>0.0054</v>
       </c>
       <c r="W11" t="n">
         <v>0.0058</v>
@@ -1327,34 +1327,34 @@
         <v>-0.1481</v>
       </c>
       <c r="N12" t="n">
-        <v>-0.0659</v>
+        <v>-0.0558</v>
       </c>
       <c r="O12" t="n">
-        <v>0.0164</v>
+        <v>0.0263</v>
       </c>
       <c r="P12" t="n">
-        <v>0.0505</v>
+        <v>0.0603</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.0466</v>
+        <v>0.0562</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.0919</v>
+        <v>-0.0922</v>
       </c>
       <c r="S12" t="n">
-        <v>-0.0868</v>
+        <v>-0.0872</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.0857</v>
+        <v>-0.086</v>
       </c>
       <c r="U12" t="n">
-        <v>-0.14</v>
+        <v>-0.1404</v>
       </c>
       <c r="V12" t="n">
-        <v>-0.0987</v>
+        <v>-0.1321</v>
       </c>
       <c r="W12" t="n">
-        <v>-6.4603</v>
+        <v>-6.5083</v>
       </c>
     </row>
     <row r="13">
@@ -1401,10 +1401,10 @@
         <v>-0.1018</v>
       </c>
       <c r="O13" t="n">
-        <v>-0.0932</v>
+        <v>-0.0933</v>
       </c>
       <c r="P13" t="n">
-        <v>-0.0551</v>
+        <v>-0.0552</v>
       </c>
       <c r="Q13" t="n">
         <v>-0.0301</v>
@@ -1422,7 +1422,7 @@
         <v>0.0001</v>
       </c>
       <c r="V13" t="n">
-        <v>-0.0001</v>
+        <v>-0.0002</v>
       </c>
       <c r="W13" t="n">
         <v>-0.0073</v>
@@ -1469,31 +1469,31 @@
         <v>-0.1408</v>
       </c>
       <c r="N14" t="n">
-        <v>-0.1042</v>
+        <v>-0.1049</v>
       </c>
       <c r="O14" t="n">
-        <v>-0.2921</v>
+        <v>-0.293</v>
       </c>
       <c r="P14" t="n">
-        <v>-0.2639</v>
+        <v>-0.2647</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.1069</v>
+        <v>-0.1076</v>
       </c>
       <c r="R14" t="n">
-        <v>-0.059</v>
+        <v>-0.0595</v>
       </c>
       <c r="S14" t="n">
-        <v>-0.0941</v>
+        <v>-0.0946</v>
       </c>
       <c r="T14" t="n">
-        <v>-0.07</v>
+        <v>-0.0705</v>
       </c>
       <c r="U14" t="n">
-        <v>-0.0316</v>
+        <v>-0.0321</v>
       </c>
       <c r="V14" t="n">
-        <v>-0.0122</v>
+        <v>-0.0129</v>
       </c>
       <c r="W14" t="n">
         <v>-0.0741</v>
@@ -1608,37 +1608,37 @@
         <v>0.5287</v>
       </c>
       <c r="M16" t="n">
-        <v>0.2312</v>
+        <v>0.2699</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.2545</v>
+        <v>-0.0284</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.7614</v>
+        <v>-0.4618</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.4572</v>
+        <v>-0.1177</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.2208</v>
+        <v>0.118</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.8013</v>
+        <v>-0.4902</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.9297</v>
+        <v>-0.6694</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.6619</v>
+        <v>-0.4286</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.4547</v>
+        <v>-0.391</v>
       </c>
       <c r="V16" t="n">
-        <v>-0.1598</v>
+        <v>-0.2829</v>
       </c>
       <c r="W16" t="n">
-        <v>-71.7788</v>
+        <v>-73.7151</v>
       </c>
     </row>
     <row r="17">
@@ -1682,34 +1682,34 @@
         <v>27957</v>
       </c>
       <c r="N17" t="n">
-        <v>28284.5</v>
+        <v>28255.9</v>
       </c>
       <c r="O17" t="n">
-        <v>28521.5094</v>
+        <v>28492.6697</v>
       </c>
       <c r="P17" t="n">
-        <v>28783.7326</v>
+        <v>28754.6278</v>
       </c>
       <c r="Q17" t="n">
-        <v>29054.2258</v>
+        <v>29024.8475</v>
       </c>
       <c r="R17" t="n">
-        <v>29343.8816</v>
+        <v>29314.2104</v>
       </c>
       <c r="S17" t="n">
-        <v>29655.9272</v>
+        <v>29625.9404</v>
       </c>
       <c r="T17" t="n">
-        <v>29972.2086</v>
+        <v>29941.9021</v>
       </c>
       <c r="U17" t="n">
-        <v>30298.979</v>
+        <v>30268.3421</v>
       </c>
       <c r="V17" t="n">
-        <v>30607.7972</v>
+        <v>30576.848</v>
       </c>
       <c r="W17" t="n">
-        <v>30918.9351</v>
+        <v>30887.6713</v>
       </c>
     </row>
     <row r="18">
@@ -1753,10 +1753,10 @@
         <v>0.1455</v>
       </c>
       <c r="N18" t="n">
-        <v>-0.1094</v>
+        <v>-0.113</v>
       </c>
       <c r="O18" t="n">
-        <v>-0.2191</v>
+        <v>-0.2194</v>
       </c>
       <c r="P18" t="n">
         <v>-0.0194</v>
@@ -1765,22 +1765,22 @@
         <v>0.0066</v>
       </c>
       <c r="R18" t="n">
-        <v>-0.3163</v>
+        <v>-0.3166</v>
       </c>
       <c r="S18" t="n">
-        <v>-0.2</v>
+        <v>-0.2002</v>
       </c>
       <c r="T18" t="n">
         <v>-0.0447</v>
       </c>
       <c r="U18" t="n">
-        <v>-0.0961</v>
+        <v>-0.0962</v>
       </c>
       <c r="V18" t="n">
-        <v>0.0004</v>
+        <v>-0.0431</v>
       </c>
       <c r="W18" t="n">
-        <v>-6.416</v>
+        <v>-6.4225</v>
       </c>
     </row>
     <row r="19">
@@ -1898,19 +1898,19 @@
         <v>-0.1124</v>
       </c>
       <c r="O20" t="n">
-        <v>-0.105</v>
+        <v>-0.1051</v>
       </c>
       <c r="P20" t="n">
-        <v>-0.1023</v>
+        <v>-0.1024</v>
       </c>
       <c r="Q20" t="n">
-        <v>-0.1004</v>
+        <v>-0.1005</v>
       </c>
       <c r="R20" t="n">
-        <v>-0.0976</v>
+        <v>-0.0977</v>
       </c>
       <c r="S20" t="n">
-        <v>-0.0948</v>
+        <v>-0.0949</v>
       </c>
       <c r="T20" t="n">
         <v>-0.001</v>
@@ -2037,34 +2037,34 @@
         <v>0.2484</v>
       </c>
       <c r="N22" t="n">
-        <v>0.0936</v>
+        <v>0.1548</v>
       </c>
       <c r="O22" t="n">
-        <v>0.1117</v>
+        <v>0.1121</v>
       </c>
       <c r="P22" t="n">
-        <v>-0.09</v>
+        <v>-0.0901</v>
       </c>
       <c r="Q22" t="n">
-        <v>-0.109</v>
+        <v>-0.1096</v>
       </c>
       <c r="R22" t="n">
         <v>0.1891</v>
       </c>
       <c r="S22" t="n">
-        <v>0.0772</v>
+        <v>0.0766</v>
       </c>
       <c r="T22" t="n">
-        <v>-0.0737</v>
+        <v>-0.0728</v>
       </c>
       <c r="U22" t="n">
-        <v>-0.0259</v>
+        <v>-0.0265</v>
       </c>
       <c r="V22" t="n">
-        <v>0.157</v>
+        <v>-0.0725</v>
       </c>
       <c r="W22" t="n">
-        <v>-37.7125</v>
+        <v>-37.8553</v>
       </c>
     </row>
     <row r="23">
@@ -2108,34 +2108,34 @@
         <v>-0.027</v>
       </c>
       <c r="N23" t="n">
-        <v>-0.02</v>
+        <v>-0.0239</v>
       </c>
       <c r="O23" t="n">
-        <v>-0.016</v>
+        <v>-0.0166</v>
       </c>
       <c r="P23" t="n">
-        <v>-0.0083</v>
+        <v>-0.009</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.0086</v>
+        <v>0.008</v>
       </c>
       <c r="R23" t="n">
-        <v>0.0231</v>
+        <v>0.0225</v>
       </c>
       <c r="S23" t="n">
-        <v>0.0026</v>
+        <v>0.002</v>
       </c>
       <c r="T23" t="n">
-        <v>0.0028</v>
+        <v>0.0022</v>
       </c>
       <c r="U23" t="n">
-        <v>0.0081</v>
+        <v>0.0075</v>
       </c>
       <c r="V23" t="n">
-        <v>0.0127</v>
+        <v>0.0125</v>
       </c>
       <c r="W23" t="n">
-        <v>0.0747</v>
+        <v>0.0753</v>
       </c>
     </row>
     <row r="24">
@@ -2179,34 +2179,34 @@
         <v>0.0574</v>
       </c>
       <c r="N24" t="n">
-        <v>0.1087</v>
+        <v>0.1796</v>
       </c>
       <c r="O24" t="n">
-        <v>0.0266</v>
+        <v>0.1009</v>
       </c>
       <c r="P24" t="n">
-        <v>-0.0298</v>
+        <v>0.047</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.0945</v>
+        <v>0.1718</v>
       </c>
       <c r="R24" t="n">
-        <v>-0.0105</v>
+        <v>-0.0012</v>
       </c>
       <c r="S24" t="n">
-        <v>-0.0245</v>
+        <v>-0.0182</v>
       </c>
       <c r="T24" t="n">
-        <v>-0.0199</v>
+        <v>-0.0156</v>
       </c>
       <c r="U24" t="n">
-        <v>-0.012</v>
+        <v>-0.0086</v>
       </c>
       <c r="V24" t="n">
-        <v>0.0007</v>
+        <v>-0.0015</v>
       </c>
       <c r="W24" t="n">
-        <v>-0.9111</v>
+        <v>-0.9989</v>
       </c>
     </row>
     <row r="25">
@@ -2250,34 +2250,34 @@
         <v>0.1388</v>
       </c>
       <c r="N25" t="n">
-        <v>0.2383</v>
+        <v>0.2521</v>
       </c>
       <c r="O25" t="n">
-        <v>0.2358</v>
+        <v>0.2497</v>
       </c>
       <c r="P25" t="n">
-        <v>0.1573</v>
+        <v>0.1642</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.1235</v>
+        <v>0.1303</v>
       </c>
       <c r="R25" t="n">
-        <v>0.0838</v>
+        <v>0.0905</v>
       </c>
       <c r="S25" t="n">
-        <v>0.011</v>
+        <v>0.0176</v>
       </c>
       <c r="T25" t="n">
-        <v>0.0411</v>
+        <v>0.0477</v>
       </c>
       <c r="U25" t="n">
-        <v>0.0515</v>
+        <v>0.0581</v>
       </c>
       <c r="V25" t="n">
-        <v>-0.0002</v>
+        <v>0.0202</v>
       </c>
       <c r="W25" t="n">
-        <v>3.9107</v>
+        <v>3.9202</v>
       </c>
     </row>
     <row r="26">
@@ -2321,7 +2321,7 @@
         <v>0.0016</v>
       </c>
       <c r="N26" t="n">
-        <v>0.009</v>
+        <v>0.0094</v>
       </c>
       <c r="O26" t="n">
         <v>0.0071</v>
@@ -2345,7 +2345,7 @@
         <v>0.0066</v>
       </c>
       <c r="V26" t="n">
-        <v>0</v>
+        <v>0.0068</v>
       </c>
       <c r="W26" t="n">
         <v>0.0067</v>
@@ -2534,19 +2534,19 @@
         <v>-0.0005</v>
       </c>
       <c r="N29" t="n">
-        <v>-0.0027</v>
+        <v>-0.003</v>
       </c>
       <c r="O29" t="n">
-        <v>0.0043</v>
+        <v>0.0044</v>
       </c>
       <c r="P29" t="n">
-        <v>0.0059</v>
+        <v>0.006</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.0055</v>
+        <v>0.0056</v>
       </c>
       <c r="R29" t="n">
-        <v>0.006</v>
+        <v>0.0061</v>
       </c>
       <c r="S29" t="n">
         <v>0.0061</v>
@@ -2558,10 +2558,10 @@
         <v>0.0021</v>
       </c>
       <c r="V29" t="n">
-        <v>0.0009</v>
+        <v>0.0006</v>
       </c>
       <c r="W29" t="n">
-        <v>-0.0727</v>
+        <v>-0.0731</v>
       </c>
     </row>
     <row r="30">
@@ -2605,7 +2605,7 @@
         <v>0</v>
       </c>
       <c r="N30" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="O30" t="n">
         <v>0</v>
@@ -2629,7 +2629,7 @@
         <v>0</v>
       </c>
       <c r="V30" t="n">
-        <v>0</v>
+        <v>0.0053</v>
       </c>
       <c r="W30" t="n">
         <v>0</v>
@@ -2679,31 +2679,31 @@
         <v>0</v>
       </c>
       <c r="O31" t="n">
-        <v>-3.775</v>
+        <v>-315.355</v>
       </c>
       <c r="P31" t="n">
-        <v>-3.466</v>
+        <v>-317.119</v>
       </c>
       <c r="Q31" t="n">
-        <v>-3.24</v>
+        <v>-318.802</v>
       </c>
       <c r="R31" t="n">
-        <v>-2.995</v>
+        <v>-320.534</v>
       </c>
       <c r="S31" t="n">
-        <v>-2.742</v>
+        <v>-322.229</v>
       </c>
       <c r="T31" t="n">
-        <v>-2.485</v>
+        <v>-323.907</v>
       </c>
       <c r="U31" t="n">
-        <v>-2.262</v>
+        <v>-325.59</v>
       </c>
       <c r="V31" t="n">
-        <v>-2.042</v>
+        <v>-327.231</v>
       </c>
       <c r="W31" t="n">
-        <v>-1.864</v>
+        <v>-328.868</v>
       </c>
     </row>
     <row r="32">
@@ -2753,7 +2753,7 @@
         <v>0</v>
       </c>
       <c r="P32" t="n">
-        <v>-0.0002</v>
+        <v>-0.0003</v>
       </c>
       <c r="Q32" t="n">
         <v>-0.0002</v>
@@ -2765,7 +2765,7 @@
         <v>-0.0003</v>
       </c>
       <c r="T32" t="n">
-        <v>-0.0003</v>
+        <v>-0.0004</v>
       </c>
       <c r="U32" t="n">
         <v>-0.0001</v>
@@ -2818,34 +2818,34 @@
         <v>0</v>
       </c>
       <c r="N33" t="n">
-        <v>0</v>
+        <v>-0.0343</v>
       </c>
       <c r="O33" t="n">
-        <v>-0.0398</v>
+        <v>-0.0393</v>
       </c>
       <c r="P33" t="n">
-        <v>-0.0413</v>
+        <v>-0.0433</v>
       </c>
       <c r="Q33" t="n">
-        <v>-0.0415</v>
+        <v>-0.0386</v>
       </c>
       <c r="R33" t="n">
-        <v>-0.0446</v>
+        <v>-0.0466</v>
       </c>
       <c r="S33" t="n">
-        <v>-0.0431</v>
+        <v>-0.0437</v>
       </c>
       <c r="T33" t="n">
-        <v>-0.0398</v>
+        <v>-0.0428</v>
       </c>
       <c r="U33" t="n">
-        <v>-0.0387</v>
+        <v>-0.0397</v>
       </c>
       <c r="V33" t="n">
-        <v>-0.0359</v>
+        <v>-0.0297</v>
       </c>
       <c r="W33" t="n">
-        <v>-0.5148</v>
+        <v>-0.7311</v>
       </c>
     </row>
     <row r="34">
@@ -2889,34 +2889,34 @@
         <v>0</v>
       </c>
       <c r="N34" t="n">
-        <v>0</v>
+        <v>-0.0082</v>
       </c>
       <c r="O34" t="n">
-        <v>-0.0018</v>
+        <v>0.0973</v>
       </c>
       <c r="P34" t="n">
-        <v>-0.0024</v>
+        <v>0.2093</v>
       </c>
       <c r="Q34" t="n">
-        <v>-0.0025</v>
+        <v>0.2012</v>
       </c>
       <c r="R34" t="n">
-        <v>-0.0032</v>
+        <v>0.267</v>
       </c>
       <c r="S34" t="n">
-        <v>-0.0026</v>
+        <v>0.2236</v>
       </c>
       <c r="T34" t="n">
-        <v>-0.0017</v>
+        <v>0.1668</v>
       </c>
       <c r="U34" t="n">
-        <v>0.0005</v>
+        <v>0.022</v>
       </c>
       <c r="V34" t="n">
-        <v>-0.0004</v>
+        <v>0.086</v>
       </c>
       <c r="W34" t="n">
-        <v>-0.0049</v>
+        <v>-1.3667</v>
       </c>
     </row>
     <row r="35">
@@ -2960,34 +2960,34 @@
         <v>0</v>
       </c>
       <c r="N35" t="n">
-        <v>0</v>
+        <v>0.0157</v>
       </c>
       <c r="O35" t="n">
-        <v>-0.006</v>
+        <v>0.0162</v>
       </c>
       <c r="P35" t="n">
-        <v>-0.0121</v>
+        <v>-0.023</v>
       </c>
       <c r="Q35" t="n">
-        <v>-0.0185</v>
+        <v>-0.0265</v>
       </c>
       <c r="R35" t="n">
-        <v>-0.0241</v>
+        <v>-0.0442</v>
       </c>
       <c r="S35" t="n">
-        <v>-0.0242</v>
+        <v>-0.048</v>
       </c>
       <c r="T35" t="n">
-        <v>-0.0241</v>
+        <v>-0.0129</v>
       </c>
       <c r="U35" t="n">
-        <v>-0.0232</v>
+        <v>-0.0158</v>
       </c>
       <c r="V35" t="n">
-        <v>-0.0218</v>
+        <v>-0.0449</v>
       </c>
       <c r="W35" t="n">
-        <v>-0.0976</v>
+        <v>-0.1266</v>
       </c>
     </row>
     <row r="36">
@@ -3028,37 +3028,37 @@
         <v>0</v>
       </c>
       <c r="M36" t="n">
-        <v>0</v>
+        <v>0.0388</v>
       </c>
       <c r="N36" t="n">
-        <v>0</v>
+        <v>0.1016</v>
       </c>
       <c r="O36" t="n">
-        <v>0.0091</v>
+        <v>0.0901</v>
       </c>
       <c r="P36" t="n">
-        <v>0.0194</v>
+        <v>0.0683</v>
       </c>
       <c r="Q36" t="n">
-        <v>0.0246</v>
+        <v>0.0728</v>
       </c>
       <c r="R36" t="n">
-        <v>0.0265</v>
+        <v>0.075</v>
       </c>
       <c r="S36" t="n">
-        <v>0.0303</v>
+        <v>0.078</v>
       </c>
       <c r="T36" t="n">
-        <v>0.0346</v>
+        <v>0.0809</v>
       </c>
       <c r="U36" t="n">
-        <v>0.0382</v>
+        <v>0.0659</v>
       </c>
       <c r="V36" t="n">
-        <v>0.0421</v>
+        <v>0.0987</v>
       </c>
       <c r="W36" t="n">
-        <v>0.154</v>
+        <v>0.098</v>
       </c>
     </row>
     <row r="37">
@@ -3108,7 +3108,7 @@
         <v>0</v>
       </c>
       <c r="P37" t="n">
-        <v>-0.0001</v>
+        <v>-0.0002</v>
       </c>
       <c r="Q37" t="n">
         <v>-0.0002</v>
@@ -3176,7 +3176,7 @@
         <v>0</v>
       </c>
       <c r="O38" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="P38" t="n">
         <v>-0.0002</v>
@@ -3191,10 +3191,10 @@
         <v>-0.0002</v>
       </c>
       <c r="T38" t="n">
-        <v>-0.0001</v>
+        <v>-0.0002</v>
       </c>
       <c r="U38" t="n">
-        <v>-0.0001</v>
+        <v>-0.0002</v>
       </c>
       <c r="V38" t="n">
         <v>-0.0001</v>
@@ -3244,7 +3244,7 @@
         <v>0</v>
       </c>
       <c r="N39" t="n">
-        <v>0</v>
+        <v>0.0011</v>
       </c>
       <c r="O39" t="n">
         <v>0</v>
@@ -3268,7 +3268,7 @@
         <v>0</v>
       </c>
       <c r="V39" t="n">
-        <v>0</v>
+        <v>0.0054</v>
       </c>
       <c r="W39" t="n">
         <v>0.0004</v>
@@ -3315,34 +3315,34 @@
         <v>0</v>
       </c>
       <c r="N40" t="n">
-        <v>0</v>
+        <v>0.0101</v>
       </c>
       <c r="O40" t="n">
-        <v>-0.0078</v>
+        <v>0.0021</v>
       </c>
       <c r="P40" t="n">
-        <v>-0.0156</v>
+        <v>-0.0059</v>
       </c>
       <c r="Q40" t="n">
-        <v>-0.0233</v>
+        <v>-0.0137</v>
       </c>
       <c r="R40" t="n">
+        <v>-0.0323</v>
+      </c>
+      <c r="S40" t="n">
+        <v>-0.0325</v>
+      </c>
+      <c r="T40" t="n">
         <v>-0.032</v>
       </c>
-      <c r="S40" t="n">
+      <c r="U40" t="n">
         <v>-0.0321</v>
       </c>
-      <c r="T40" t="n">
-        <v>-0.0317</v>
-      </c>
-      <c r="U40" t="n">
-        <v>-0.0317</v>
-      </c>
       <c r="V40" t="n">
-        <v>-0.03</v>
+        <v>-0.0634</v>
       </c>
       <c r="W40" t="n">
-        <v>-0.1228</v>
+        <v>-0.1708</v>
       </c>
     </row>
     <row r="41">
@@ -3389,10 +3389,10 @@
         <v>0</v>
       </c>
       <c r="O41" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="P41" t="n">
-        <v>-0.0002</v>
+        <v>-0.0003</v>
       </c>
       <c r="Q41" t="n">
         <v>-0.0002</v>
@@ -3410,10 +3410,10 @@
         <v>0</v>
       </c>
       <c r="V41" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="W41" t="n">
-        <v>-0.0001</v>
+        <v>-0.0002</v>
       </c>
     </row>
     <row r="42">
@@ -3457,31 +3457,31 @@
         <v>0</v>
       </c>
       <c r="N42" t="n">
-        <v>0</v>
+        <v>-0.0007</v>
       </c>
       <c r="O42" t="n">
-        <v>-0.0001</v>
+        <v>-0.001</v>
       </c>
       <c r="P42" t="n">
-        <v>-0.0011</v>
+        <v>-0.0019</v>
       </c>
       <c r="Q42" t="n">
-        <v>-0.0009</v>
+        <v>-0.0015</v>
       </c>
       <c r="R42" t="n">
-        <v>-0.0008</v>
+        <v>-0.0013</v>
       </c>
       <c r="S42" t="n">
-        <v>-0.0014</v>
+        <v>-0.0019</v>
       </c>
       <c r="T42" t="n">
+        <v>-0.0018</v>
+      </c>
+      <c r="U42" t="n">
         <v>-0.0013</v>
       </c>
-      <c r="U42" t="n">
-        <v>-0.0009</v>
-      </c>
       <c r="V42" t="n">
-        <v>-0.0006</v>
+        <v>-0.0013</v>
       </c>
       <c r="W42" t="n">
         <v>-0.0016</v>
@@ -3596,37 +3596,37 @@
         <v>0</v>
       </c>
       <c r="M44" t="n">
-        <v>0</v>
+        <v>0.0388</v>
       </c>
       <c r="N44" t="n">
-        <v>0</v>
+        <v>0.226</v>
       </c>
       <c r="O44" t="n">
-        <v>-0.0876</v>
+        <v>0.2121</v>
       </c>
       <c r="P44" t="n">
-        <v>-0.0942</v>
+        <v>0.2453</v>
       </c>
       <c r="Q44" t="n">
-        <v>-0.1018</v>
+        <v>0.237</v>
       </c>
       <c r="R44" t="n">
-        <v>-0.1151</v>
+        <v>0.196</v>
       </c>
       <c r="S44" t="n">
-        <v>-0.1102</v>
+        <v>0.1501</v>
       </c>
       <c r="T44" t="n">
-        <v>-0.0977</v>
+        <v>0.1356</v>
       </c>
       <c r="U44" t="n">
-        <v>-0.0843</v>
+        <v>-0.0205</v>
       </c>
       <c r="V44" t="n">
-        <v>-0.0689</v>
+        <v>-0.192</v>
       </c>
       <c r="W44" t="n">
-        <v>-1.1317</v>
+        <v>-3.068</v>
       </c>
     </row>
     <row r="45">
@@ -3670,34 +3670,34 @@
         <v>0</v>
       </c>
       <c r="N45" t="n">
-        <v>0</v>
+        <v>-28.6</v>
       </c>
       <c r="O45" t="n">
-        <v>-100.9646</v>
+        <v>-129.8043</v>
       </c>
       <c r="P45" t="n">
-        <v>-183.6044</v>
+        <v>-212.7092</v>
       </c>
       <c r="Q45" t="n">
-        <v>-270.1862</v>
+        <v>-299.5645</v>
       </c>
       <c r="R45" t="n">
-        <v>-344.39</v>
+        <v>-374.0612</v>
       </c>
       <c r="S45" t="n">
-        <v>-387.5407</v>
+        <v>-417.5275</v>
       </c>
       <c r="T45" t="n">
-        <v>-421.4454</v>
+        <v>-451.7519</v>
       </c>
       <c r="U45" t="n">
-        <v>-432.3359</v>
+        <v>-462.9728</v>
       </c>
       <c r="V45" t="n">
-        <v>-461.3873</v>
+        <v>-492.3365</v>
       </c>
       <c r="W45" t="n">
-        <v>-493.0248</v>
+        <v>-524.2886</v>
       </c>
     </row>
     <row r="46">
@@ -3741,10 +3741,10 @@
         <v>0</v>
       </c>
       <c r="N46" t="n">
-        <v>0</v>
+        <v>-0.0036</v>
       </c>
       <c r="O46" t="n">
-        <v>-0.0086</v>
+        <v>-0.0088</v>
       </c>
       <c r="P46" t="n">
         <v>-0.0087</v>
@@ -3753,10 +3753,10 @@
         <v>-0.0086</v>
       </c>
       <c r="R46" t="n">
-        <v>-0.0115</v>
+        <v>-0.0118</v>
       </c>
       <c r="S46" t="n">
-        <v>-0.0104</v>
+        <v>-0.0106</v>
       </c>
       <c r="T46" t="n">
         <v>-0.0082</v>
@@ -3765,10 +3765,10 @@
         <v>-0.0086</v>
       </c>
       <c r="V46" t="n">
-        <v>-0.0068</v>
+        <v>-0.0503</v>
       </c>
       <c r="W46" t="n">
-        <v>-0.1009</v>
+        <v>-0.1074</v>
       </c>
     </row>
     <row r="47">
@@ -3886,19 +3886,19 @@
         <v>0</v>
       </c>
       <c r="O48" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="P48" t="n">
-        <v>-0.0004</v>
+        <v>-0.0005</v>
       </c>
       <c r="Q48" t="n">
-        <v>-0.0006</v>
+        <v>-0.0007</v>
       </c>
       <c r="R48" t="n">
-        <v>-0.0009</v>
+        <v>-0.001</v>
       </c>
       <c r="S48" t="n">
-        <v>-0.0011</v>
+        <v>-0.0012</v>
       </c>
       <c r="T48" t="n">
         <v>0</v>
@@ -4025,34 +4025,34 @@
         <v>0</v>
       </c>
       <c r="N50" t="n">
-        <v>0</v>
+        <v>0.0612</v>
       </c>
       <c r="O50" t="n">
-        <v>-0.044</v>
+        <v>-0.0437</v>
       </c>
       <c r="P50" t="n">
-        <v>-0.0463</v>
+        <v>-0.0464</v>
       </c>
       <c r="Q50" t="n">
-        <v>-0.0464</v>
+        <v>-0.0471</v>
       </c>
       <c r="R50" t="n">
         <v>-0.0435</v>
       </c>
       <c r="S50" t="n">
-        <v>-0.0439</v>
+        <v>-0.0445</v>
       </c>
       <c r="T50" t="n">
-        <v>-0.0446</v>
+        <v>-0.0437</v>
       </c>
       <c r="U50" t="n">
-        <v>-0.042</v>
+        <v>-0.0426</v>
       </c>
       <c r="V50" t="n">
-        <v>-0.0374</v>
+        <v>-0.2669</v>
       </c>
       <c r="W50" t="n">
-        <v>-0.5934</v>
+        <v>-0.7361</v>
       </c>
     </row>
     <row r="51">
@@ -4096,34 +4096,34 @@
         <v>0</v>
       </c>
       <c r="N51" t="n">
-        <v>0</v>
+        <v>-0.0039</v>
       </c>
       <c r="O51" t="n">
+        <v>-0.0006</v>
+      </c>
+      <c r="P51" t="n">
+        <v>-0.0005</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>-0.0003</v>
+      </c>
+      <c r="R51" t="n">
+        <v>0</v>
+      </c>
+      <c r="S51" t="n">
+        <v>-0.0001</v>
+      </c>
+      <c r="T51" t="n">
+        <v>-0.0001</v>
+      </c>
+      <c r="U51" t="n">
         <v>0.0001</v>
       </c>
-      <c r="P51" t="n">
-        <v>0.0002</v>
-      </c>
-      <c r="Q51" t="n">
-        <v>0.0003</v>
-      </c>
-      <c r="R51" t="n">
+      <c r="V51" t="n">
         <v>0.0006</v>
       </c>
-      <c r="S51" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="T51" t="n">
-        <v>0.0006</v>
-      </c>
-      <c r="U51" t="n">
-        <v>0.0007</v>
-      </c>
-      <c r="V51" t="n">
-        <v>0.0008</v>
-      </c>
       <c r="W51" t="n">
-        <v>0.0018</v>
+        <v>0.0024</v>
       </c>
     </row>
     <row r="52">
@@ -4167,34 +4167,34 @@
         <v>0</v>
       </c>
       <c r="N52" t="n">
-        <v>0</v>
+        <v>0.071</v>
       </c>
       <c r="O52" t="n">
-        <v>-0.0011</v>
+        <v>0.0733</v>
       </c>
       <c r="P52" t="n">
-        <v>-0.0023</v>
+        <v>0.0745</v>
       </c>
       <c r="Q52" t="n">
-        <v>-0.0027</v>
+        <v>0.0746</v>
       </c>
       <c r="R52" t="n">
-        <v>-0.0045</v>
+        <v>0.0048</v>
       </c>
       <c r="S52" t="n">
-        <v>-0.0047</v>
+        <v>0.0016</v>
       </c>
       <c r="T52" t="n">
-        <v>-0.0046</v>
+        <v>-0.0003</v>
       </c>
       <c r="U52" t="n">
-        <v>-0.0044</v>
+        <v>-0.0009</v>
       </c>
       <c r="V52" t="n">
-        <v>-0.004</v>
+        <v>-0.0062</v>
       </c>
       <c r="W52" t="n">
-        <v>-0.0173</v>
+        <v>-0.1052</v>
       </c>
     </row>
     <row r="53">
@@ -4238,34 +4238,34 @@
         <v>0</v>
       </c>
       <c r="N53" t="n">
-        <v>0</v>
+        <v>0.0137</v>
       </c>
       <c r="O53" t="n">
-        <v>0.0046</v>
+        <v>0.0185</v>
       </c>
       <c r="P53" t="n">
-        <v>0.01</v>
+        <v>0.0169</v>
       </c>
       <c r="Q53" t="n">
-        <v>0.0126</v>
+        <v>0.0194</v>
       </c>
       <c r="R53" t="n">
-        <v>0.0149</v>
+        <v>0.0216</v>
       </c>
       <c r="S53" t="n">
-        <v>0.0164</v>
+        <v>0.023</v>
       </c>
       <c r="T53" t="n">
-        <v>0.0188</v>
+        <v>0.0254</v>
       </c>
       <c r="U53" t="n">
-        <v>0.0209</v>
+        <v>0.0274</v>
       </c>
       <c r="V53" t="n">
-        <v>0.0218</v>
+        <v>0.0423</v>
       </c>
       <c r="W53" t="n">
-        <v>0.0791</v>
+        <v>0.0886</v>
       </c>
     </row>
     <row r="54">
@@ -4309,7 +4309,7 @@
         <v>0</v>
       </c>
       <c r="N54" t="n">
-        <v>0</v>
+        <v>0.0005</v>
       </c>
       <c r="O54" t="n">
         <v>0</v>
@@ -4333,7 +4333,7 @@
         <v>0</v>
       </c>
       <c r="V54" t="n">
-        <v>0</v>
+        <v>0.0068</v>
       </c>
       <c r="W54" t="n">
         <v>-0.0001</v>
@@ -4522,10 +4522,10 @@
         <v>0</v>
       </c>
       <c r="N57" t="n">
-        <v>0</v>
+        <v>-0.0003</v>
       </c>
       <c r="O57" t="n">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
       <c r="P57" t="n">
         <v>-0.0001</v>
@@ -4534,10 +4534,10 @@
         <v>-0.0002</v>
       </c>
       <c r="R57" t="n">
+        <v>-0.0001</v>
+      </c>
+      <c r="S57" t="n">
         <v>-0.0002</v>
-      </c>
-      <c r="S57" t="n">
-        <v>-0.0003</v>
       </c>
       <c r="T57" t="n">
         <v>-0.0003</v>
@@ -4546,10 +4546,10 @@
         <v>-0.0003</v>
       </c>
       <c r="V57" t="n">
-        <v>-0.0004</v>
+        <v>-0.0007</v>
       </c>
       <c r="W57" t="n">
-        <v>-0.0014</v>
+        <v>-0.0018</v>
       </c>
     </row>
     <row r="58">

</xml_diff>

<commit_message>
FIM run and forecast pull forward
</commit_message>
<xml_diff>
--- a/results/05-2024/comparison-deflators-05-2024.xlsx
+++ b/results/05-2024/comparison-deflators-05-2024.xlsx
@@ -620,13 +620,13 @@
         <v>0.0082</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0067</v>
+        <v>0.0085</v>
       </c>
       <c r="P2" t="n">
-        <v>0.006</v>
+        <v>0.0071</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.0055</v>
+        <v>0.0062</v>
       </c>
       <c r="R2" t="n">
         <v>0.0056</v>
@@ -833,13 +833,13 @@
         <v>-0.3011</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.3991</v>
+        <v>-0.4557</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.1106</v>
+        <v>-0.1629</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.1223</v>
+        <v>-0.1465</v>
       </c>
       <c r="R5" t="n">
         <v>-0.4687</v>
@@ -904,31 +904,31 @@
         <v>0.1478</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.023</v>
+        <v>-0.0256</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.0289</v>
+        <v>-0.0302</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.0223</v>
+        <v>-0.0229</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.0168</v>
+        <v>-0.0161</v>
       </c>
       <c r="S6" t="n">
-        <v>0.0041</v>
+        <v>0.0049</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.0039</v>
+        <v>-0.0031</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.0134</v>
+        <v>-0.0127</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.0281</v>
+        <v>-0.0274</v>
       </c>
       <c r="W6" t="n">
-        <v>-1.794</v>
+        <v>-1.7933</v>
       </c>
     </row>
     <row r="7">
@@ -975,31 +975,31 @@
         <v>-0.2068</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.167</v>
+        <v>-0.1279</v>
       </c>
       <c r="P7" t="n">
-        <v>0.0162</v>
+        <v>0.0584</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.0276</v>
+        <v>0.0104</v>
       </c>
       <c r="R7" t="n">
-        <v>0.0109</v>
+        <v>0.0486</v>
       </c>
       <c r="S7" t="n">
-        <v>-0.0032</v>
+        <v>-0.0036</v>
       </c>
       <c r="T7" t="n">
-        <v>0.0192</v>
+        <v>0.0157</v>
       </c>
       <c r="U7" t="n">
-        <v>0.0327</v>
+        <v>0.033</v>
       </c>
       <c r="V7" t="n">
-        <v>0.0471</v>
+        <v>0.0476</v>
       </c>
       <c r="W7" t="n">
-        <v>-5.1508</v>
+        <v>-5.2081</v>
       </c>
     </row>
     <row r="8">
@@ -1046,31 +1046,31 @@
         <v>0.303</v>
       </c>
       <c r="O8" t="n">
-        <v>0.2001</v>
+        <v>0.1788</v>
       </c>
       <c r="P8" t="n">
-        <v>0.3412</v>
+        <v>0.3287</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.2815</v>
+        <v>0.2853</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.0589</v>
+        <v>-0.0597</v>
       </c>
       <c r="S8" t="n">
-        <v>-0.0737</v>
+        <v>-0.0771</v>
       </c>
       <c r="T8" t="n">
-        <v>-0.0432</v>
+        <v>-0.046</v>
       </c>
       <c r="U8" t="n">
-        <v>-0.0514</v>
+        <v>-0.0541</v>
       </c>
       <c r="V8" t="n">
-        <v>0.0313</v>
+        <v>0.0282</v>
       </c>
       <c r="W8" t="n">
-        <v>7.5608</v>
+        <v>7.6011</v>
       </c>
     </row>
     <row r="9">
@@ -1129,7 +1129,7 @@
         <v>-0.0154</v>
       </c>
       <c r="S9" t="n">
-        <v>-0.0139</v>
+        <v>-0.014</v>
       </c>
       <c r="T9" t="n">
         <v>-0.0141</v>
@@ -1200,16 +1200,16 @@
         <v>-0.0104</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.0099</v>
+        <v>-0.01</v>
       </c>
       <c r="T10" t="n">
         <v>-0.0084</v>
       </c>
       <c r="U10" t="n">
-        <v>-0.0076</v>
+        <v>-0.0077</v>
       </c>
       <c r="V10" t="n">
-        <v>-0.007</v>
+        <v>-0.0071</v>
       </c>
       <c r="W10" t="n">
         <v>-0.0065</v>
@@ -1259,13 +1259,13 @@
         <v>0.0112</v>
       </c>
       <c r="O11" t="n">
-        <v>0.0078</v>
+        <v>0.0095</v>
       </c>
       <c r="P11" t="n">
-        <v>0.0066</v>
+        <v>0.0082</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.007</v>
+        <v>0.0077</v>
       </c>
       <c r="R11" t="n">
         <v>0.0064</v>
@@ -1330,22 +1330,22 @@
         <v>-0.0558</v>
       </c>
       <c r="O12" t="n">
-        <v>0.0263</v>
+        <v>0.0152</v>
       </c>
       <c r="P12" t="n">
-        <v>0.0603</v>
+        <v>0.0421</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.0562</v>
+        <v>0.0334</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.0922</v>
+        <v>-0.1148</v>
       </c>
       <c r="S12" t="n">
-        <v>-0.0872</v>
+        <v>-0.0988</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.086</v>
+        <v>-0.0906</v>
       </c>
       <c r="U12" t="n">
         <v>-0.1404</v>
@@ -1413,7 +1413,7 @@
         <v>-0.0298</v>
       </c>
       <c r="S13" t="n">
-        <v>-0.0235</v>
+        <v>-0.0236</v>
       </c>
       <c r="T13" t="n">
         <v>0.0002</v>
@@ -1472,31 +1472,31 @@
         <v>-0.1049</v>
       </c>
       <c r="O14" t="n">
-        <v>-0.293</v>
+        <v>-0.2931</v>
       </c>
       <c r="P14" t="n">
-        <v>-0.2647</v>
+        <v>-0.2649</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.1076</v>
+        <v>-0.1078</v>
       </c>
       <c r="R14" t="n">
-        <v>-0.0595</v>
+        <v>-0.0597</v>
       </c>
       <c r="S14" t="n">
-        <v>-0.0946</v>
+        <v>-0.0948</v>
       </c>
       <c r="T14" t="n">
-        <v>-0.0705</v>
+        <v>-0.0707</v>
       </c>
       <c r="U14" t="n">
-        <v>-0.0321</v>
+        <v>-0.0322</v>
       </c>
       <c r="V14" t="n">
-        <v>-0.0129</v>
+        <v>-0.0131</v>
       </c>
       <c r="W14" t="n">
-        <v>-0.0741</v>
+        <v>-0.0742</v>
       </c>
     </row>
     <row r="15">
@@ -1614,31 +1614,31 @@
         <v>-0.0284</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.4618</v>
+        <v>-0.5629</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.1177</v>
+        <v>-0.2064</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.118</v>
+        <v>0.094</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.4902</v>
+        <v>-0.4702</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.6694</v>
+        <v>-0.6931</v>
       </c>
       <c r="T16" t="n">
-        <v>-0.4286</v>
+        <v>-0.4406</v>
       </c>
       <c r="U16" t="n">
-        <v>-0.391</v>
+        <v>-0.3915</v>
       </c>
       <c r="V16" t="n">
-        <v>-0.2829</v>
+        <v>-0.282</v>
       </c>
       <c r="W16" t="n">
-        <v>-73.7151</v>
+        <v>-73.7292</v>
       </c>
     </row>
     <row r="17">
@@ -1756,13 +1756,13 @@
         <v>-0.113</v>
       </c>
       <c r="O18" t="n">
-        <v>-0.2194</v>
+        <v>-0.2316</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.0194</v>
+        <v>-0.0305</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.0066</v>
+        <v>0.0015</v>
       </c>
       <c r="R18" t="n">
         <v>-0.3166</v>
@@ -2040,13 +2040,13 @@
         <v>0.1548</v>
       </c>
       <c r="O22" t="n">
-        <v>0.1121</v>
+        <v>0.0493</v>
       </c>
       <c r="P22" t="n">
-        <v>-0.0901</v>
+        <v>-0.1489</v>
       </c>
       <c r="Q22" t="n">
-        <v>-0.1096</v>
+        <v>-0.1368</v>
       </c>
       <c r="R22" t="n">
         <v>0.1891</v>
@@ -2111,31 +2111,31 @@
         <v>-0.0239</v>
       </c>
       <c r="O23" t="n">
-        <v>-0.0166</v>
+        <v>-0.0165</v>
       </c>
       <c r="P23" t="n">
-        <v>-0.009</v>
+        <v>-0.0088</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.008</v>
+        <v>0.0082</v>
       </c>
       <c r="R23" t="n">
-        <v>0.0225</v>
+        <v>0.0227</v>
       </c>
       <c r="S23" t="n">
-        <v>0.002</v>
+        <v>0.0023</v>
       </c>
       <c r="T23" t="n">
-        <v>0.0022</v>
+        <v>0.0025</v>
       </c>
       <c r="U23" t="n">
-        <v>0.0075</v>
+        <v>0.0078</v>
       </c>
       <c r="V23" t="n">
-        <v>0.0125</v>
+        <v>0.0127</v>
       </c>
       <c r="W23" t="n">
-        <v>0.0753</v>
+        <v>0.0755</v>
       </c>
     </row>
     <row r="24">
@@ -2182,31 +2182,31 @@
         <v>0.1796</v>
       </c>
       <c r="O24" t="n">
-        <v>0.1009</v>
+        <v>0.1152</v>
       </c>
       <c r="P24" t="n">
-        <v>0.047</v>
+        <v>0.0565</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.1718</v>
+        <v>0.1805</v>
       </c>
       <c r="R24" t="n">
-        <v>-0.0012</v>
+        <v>0.0073</v>
       </c>
       <c r="S24" t="n">
-        <v>-0.0182</v>
+        <v>-0.0236</v>
       </c>
       <c r="T24" t="n">
-        <v>-0.0156</v>
+        <v>-0.0165</v>
       </c>
       <c r="U24" t="n">
-        <v>-0.0086</v>
+        <v>-0.0087</v>
       </c>
       <c r="V24" t="n">
         <v>-0.0015</v>
       </c>
       <c r="W24" t="n">
-        <v>-0.9989</v>
+        <v>-1.0114</v>
       </c>
     </row>
     <row r="25">
@@ -2253,31 +2253,31 @@
         <v>0.2521</v>
       </c>
       <c r="O25" t="n">
-        <v>0.2497</v>
+        <v>0.2563</v>
       </c>
       <c r="P25" t="n">
-        <v>0.1642</v>
+        <v>0.175</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.1303</v>
+        <v>0.1406</v>
       </c>
       <c r="R25" t="n">
-        <v>0.0905</v>
+        <v>0.0987</v>
       </c>
       <c r="S25" t="n">
-        <v>0.0176</v>
+        <v>0.0243</v>
       </c>
       <c r="T25" t="n">
-        <v>0.0477</v>
+        <v>0.0542</v>
       </c>
       <c r="U25" t="n">
-        <v>0.0581</v>
+        <v>0.0646</v>
       </c>
       <c r="V25" t="n">
-        <v>0.0202</v>
+        <v>0.0267</v>
       </c>
       <c r="W25" t="n">
-        <v>3.9202</v>
+        <v>3.9236</v>
       </c>
     </row>
     <row r="26">
@@ -2324,13 +2324,13 @@
         <v>0.0094</v>
       </c>
       <c r="O26" t="n">
-        <v>0.0071</v>
+        <v>0.0088</v>
       </c>
       <c r="P26" t="n">
-        <v>0.0064</v>
+        <v>0.008</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.0063</v>
+        <v>0.007</v>
       </c>
       <c r="R26" t="n">
         <v>0.0066</v>
@@ -2537,31 +2537,31 @@
         <v>-0.003</v>
       </c>
       <c r="O29" t="n">
-        <v>0.0044</v>
+        <v>-0.0014</v>
       </c>
       <c r="P29" t="n">
-        <v>0.006</v>
+        <v>-0.0003</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.0056</v>
+        <v>-0.0025</v>
       </c>
       <c r="R29" t="n">
-        <v>0.0061</v>
+        <v>-0.0034</v>
       </c>
       <c r="S29" t="n">
-        <v>0.0061</v>
+        <v>-0.0031</v>
       </c>
       <c r="T29" t="n">
-        <v>0.0046</v>
+        <v>-0.0024</v>
       </c>
       <c r="U29" t="n">
-        <v>0.0021</v>
+        <v>-0.0033</v>
       </c>
       <c r="V29" t="n">
-        <v>0.0006</v>
+        <v>-0.0031</v>
       </c>
       <c r="W29" t="n">
-        <v>-0.0731</v>
+        <v>-0.0618</v>
       </c>
     </row>
     <row r="30">
@@ -2608,13 +2608,13 @@
         <v>-0.0002</v>
       </c>
       <c r="O30" t="n">
-        <v>0</v>
+        <v>0.0017</v>
       </c>
       <c r="P30" t="n">
-        <v>0</v>
+        <v>0.0011</v>
       </c>
       <c r="Q30" t="n">
-        <v>0</v>
+        <v>0.0007</v>
       </c>
       <c r="R30" t="n">
         <v>0</v>
@@ -2821,13 +2821,13 @@
         <v>-0.0343</v>
       </c>
       <c r="O33" t="n">
-        <v>-0.0393</v>
+        <v>-0.0959</v>
       </c>
       <c r="P33" t="n">
-        <v>-0.0433</v>
+        <v>-0.0956</v>
       </c>
       <c r="Q33" t="n">
-        <v>-0.0386</v>
+        <v>-0.0627</v>
       </c>
       <c r="R33" t="n">
         <v>-0.0466</v>
@@ -2892,31 +2892,31 @@
         <v>-0.0082</v>
       </c>
       <c r="O34" t="n">
-        <v>0.0973</v>
+        <v>0.0947</v>
       </c>
       <c r="P34" t="n">
-        <v>0.2093</v>
+        <v>0.2079</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.2012</v>
+        <v>0.2006</v>
       </c>
       <c r="R34" t="n">
-        <v>0.267</v>
+        <v>0.2678</v>
       </c>
       <c r="S34" t="n">
-        <v>0.2236</v>
+        <v>0.2243</v>
       </c>
       <c r="T34" t="n">
-        <v>0.1668</v>
+        <v>0.1675</v>
       </c>
       <c r="U34" t="n">
-        <v>0.022</v>
+        <v>0.0227</v>
       </c>
       <c r="V34" t="n">
-        <v>0.086</v>
+        <v>0.0867</v>
       </c>
       <c r="W34" t="n">
-        <v>-1.3667</v>
+        <v>-1.366</v>
       </c>
     </row>
     <row r="35">
@@ -2963,31 +2963,31 @@
         <v>0.0157</v>
       </c>
       <c r="O35" t="n">
-        <v>0.0162</v>
+        <v>0.0553</v>
       </c>
       <c r="P35" t="n">
-        <v>-0.023</v>
+        <v>0.0191</v>
       </c>
       <c r="Q35" t="n">
-        <v>-0.0265</v>
+        <v>0.0115</v>
       </c>
       <c r="R35" t="n">
-        <v>-0.0442</v>
+        <v>-0.0065</v>
       </c>
       <c r="S35" t="n">
-        <v>-0.048</v>
+        <v>-0.0484</v>
       </c>
       <c r="T35" t="n">
-        <v>-0.0129</v>
+        <v>-0.0164</v>
       </c>
       <c r="U35" t="n">
-        <v>-0.0158</v>
+        <v>-0.0155</v>
       </c>
       <c r="V35" t="n">
-        <v>-0.0449</v>
+        <v>-0.0444</v>
       </c>
       <c r="W35" t="n">
-        <v>-0.1266</v>
+        <v>-0.1839</v>
       </c>
     </row>
     <row r="36">
@@ -3034,31 +3034,31 @@
         <v>0.1016</v>
       </c>
       <c r="O36" t="n">
-        <v>0.0901</v>
+        <v>0.0688</v>
       </c>
       <c r="P36" t="n">
-        <v>0.0683</v>
+        <v>0.0558</v>
       </c>
       <c r="Q36" t="n">
-        <v>0.0728</v>
+        <v>0.0767</v>
       </c>
       <c r="R36" t="n">
-        <v>0.075</v>
+        <v>0.0741</v>
       </c>
       <c r="S36" t="n">
-        <v>0.078</v>
+        <v>0.0746</v>
       </c>
       <c r="T36" t="n">
-        <v>0.0809</v>
+        <v>0.0781</v>
       </c>
       <c r="U36" t="n">
-        <v>0.0659</v>
+        <v>0.0633</v>
       </c>
       <c r="V36" t="n">
-        <v>0.0987</v>
+        <v>0.0956</v>
       </c>
       <c r="W36" t="n">
-        <v>0.098</v>
+        <v>0.1382</v>
       </c>
     </row>
     <row r="37">
@@ -3126,7 +3126,7 @@
         <v>-0.0002</v>
       </c>
       <c r="V37" t="n">
-        <v>-0.0002</v>
+        <v>-0.0003</v>
       </c>
       <c r="W37" t="n">
         <v>-0.0002</v>
@@ -3179,13 +3179,13 @@
         <v>-0.0001</v>
       </c>
       <c r="P38" t="n">
+        <v>-0.0003</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>-0.0003</v>
+      </c>
+      <c r="R38" t="n">
         <v>-0.0002</v>
-      </c>
-      <c r="Q38" t="n">
-        <v>-0.0002</v>
-      </c>
-      <c r="R38" t="n">
-        <v>-0.0001</v>
       </c>
       <c r="S38" t="n">
         <v>-0.0002</v>
@@ -3197,7 +3197,7 @@
         <v>-0.0002</v>
       </c>
       <c r="V38" t="n">
-        <v>-0.0001</v>
+        <v>-0.0002</v>
       </c>
       <c r="W38" t="n">
         <v>-0.0001</v>
@@ -3247,13 +3247,13 @@
         <v>0.0011</v>
       </c>
       <c r="O39" t="n">
-        <v>0</v>
+        <v>0.0017</v>
       </c>
       <c r="P39" t="n">
-        <v>0</v>
+        <v>0.0016</v>
       </c>
       <c r="Q39" t="n">
-        <v>0</v>
+        <v>0.0007</v>
       </c>
       <c r="R39" t="n">
         <v>0</v>
@@ -3318,22 +3318,22 @@
         <v>0.0101</v>
       </c>
       <c r="O40" t="n">
-        <v>0.0021</v>
+        <v>-0.0091</v>
       </c>
       <c r="P40" t="n">
-        <v>-0.0059</v>
+        <v>-0.0241</v>
       </c>
       <c r="Q40" t="n">
-        <v>-0.0137</v>
+        <v>-0.0365</v>
       </c>
       <c r="R40" t="n">
-        <v>-0.0323</v>
+        <v>-0.0549</v>
       </c>
       <c r="S40" t="n">
-        <v>-0.0325</v>
+        <v>-0.0441</v>
       </c>
       <c r="T40" t="n">
-        <v>-0.032</v>
+        <v>-0.0366</v>
       </c>
       <c r="U40" t="n">
         <v>-0.0321</v>
@@ -3395,10 +3395,10 @@
         <v>-0.0003</v>
       </c>
       <c r="Q41" t="n">
-        <v>-0.0002</v>
+        <v>-0.0003</v>
       </c>
       <c r="R41" t="n">
-        <v>-0.0003</v>
+        <v>-0.0004</v>
       </c>
       <c r="S41" t="n">
         <v>-0.0003</v>
@@ -3460,31 +3460,31 @@
         <v>-0.0007</v>
       </c>
       <c r="O42" t="n">
-        <v>-0.001</v>
+        <v>-0.0011</v>
       </c>
       <c r="P42" t="n">
+        <v>-0.0021</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>-0.0017</v>
+      </c>
+      <c r="R42" t="n">
+        <v>-0.0015</v>
+      </c>
+      <c r="S42" t="n">
+        <v>-0.0021</v>
+      </c>
+      <c r="T42" t="n">
         <v>-0.0019</v>
       </c>
-      <c r="Q42" t="n">
+      <c r="U42" t="n">
         <v>-0.0015</v>
       </c>
-      <c r="R42" t="n">
-        <v>-0.0013</v>
-      </c>
-      <c r="S42" t="n">
-        <v>-0.0019</v>
-      </c>
-      <c r="T42" t="n">
+      <c r="V42" t="n">
+        <v>-0.0015</v>
+      </c>
+      <c r="W42" t="n">
         <v>-0.0018</v>
-      </c>
-      <c r="U42" t="n">
-        <v>-0.0013</v>
-      </c>
-      <c r="V42" t="n">
-        <v>-0.0013</v>
-      </c>
-      <c r="W42" t="n">
-        <v>-0.0016</v>
       </c>
     </row>
     <row r="43">
@@ -3602,31 +3602,31 @@
         <v>0.226</v>
       </c>
       <c r="O44" t="n">
-        <v>0.2121</v>
+        <v>0.1109</v>
       </c>
       <c r="P44" t="n">
-        <v>0.2453</v>
+        <v>0.1567</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.237</v>
+        <v>0.213</v>
       </c>
       <c r="R44" t="n">
-        <v>0.196</v>
+        <v>0.2161</v>
       </c>
       <c r="S44" t="n">
-        <v>0.1501</v>
+        <v>0.1264</v>
       </c>
       <c r="T44" t="n">
-        <v>0.1356</v>
+        <v>0.1236</v>
       </c>
       <c r="U44" t="n">
-        <v>-0.0205</v>
+        <v>-0.021</v>
       </c>
       <c r="V44" t="n">
-        <v>-0.192</v>
+        <v>-0.1911</v>
       </c>
       <c r="W44" t="n">
-        <v>-3.068</v>
+        <v>-3.082</v>
       </c>
     </row>
     <row r="45">
@@ -3744,13 +3744,13 @@
         <v>-0.0036</v>
       </c>
       <c r="O46" t="n">
-        <v>-0.0088</v>
+        <v>-0.021</v>
       </c>
       <c r="P46" t="n">
-        <v>-0.0087</v>
+        <v>-0.0198</v>
       </c>
       <c r="Q46" t="n">
-        <v>-0.0086</v>
+        <v>-0.0137</v>
       </c>
       <c r="R46" t="n">
         <v>-0.0118</v>
@@ -4028,13 +4028,13 @@
         <v>0.0612</v>
       </c>
       <c r="O50" t="n">
-        <v>-0.0437</v>
+        <v>-0.1065</v>
       </c>
       <c r="P50" t="n">
-        <v>-0.0464</v>
+        <v>-0.1052</v>
       </c>
       <c r="Q50" t="n">
-        <v>-0.0471</v>
+        <v>-0.0743</v>
       </c>
       <c r="R50" t="n">
         <v>-0.0435</v>
@@ -4099,31 +4099,31 @@
         <v>-0.0039</v>
       </c>
       <c r="O51" t="n">
-        <v>-0.0006</v>
+        <v>-0.0004</v>
       </c>
       <c r="P51" t="n">
-        <v>-0.0005</v>
+        <v>-0.0003</v>
       </c>
       <c r="Q51" t="n">
-        <v>-0.0003</v>
+        <v>0</v>
       </c>
       <c r="R51" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="S51" t="n">
-        <v>-0.0001</v>
+        <v>0.0001</v>
       </c>
       <c r="T51" t="n">
-        <v>-0.0001</v>
+        <v>0.0002</v>
       </c>
       <c r="U51" t="n">
-        <v>0.0001</v>
+        <v>0.0004</v>
       </c>
       <c r="V51" t="n">
-        <v>0.0006</v>
+        <v>0.0009</v>
       </c>
       <c r="W51" t="n">
-        <v>0.0024</v>
+        <v>0.0026</v>
       </c>
     </row>
     <row r="52">
@@ -4170,31 +4170,31 @@
         <v>0.071</v>
       </c>
       <c r="O52" t="n">
-        <v>0.0733</v>
+        <v>0.0876</v>
       </c>
       <c r="P52" t="n">
-        <v>0.0745</v>
+        <v>0.084</v>
       </c>
       <c r="Q52" t="n">
-        <v>0.0746</v>
+        <v>0.0833</v>
       </c>
       <c r="R52" t="n">
-        <v>0.0048</v>
+        <v>0.0133</v>
       </c>
       <c r="S52" t="n">
-        <v>0.0016</v>
+        <v>-0.0038</v>
       </c>
       <c r="T52" t="n">
-        <v>-0.0003</v>
+        <v>-0.0012</v>
       </c>
       <c r="U52" t="n">
-        <v>-0.0009</v>
+        <v>-0.0011</v>
       </c>
       <c r="V52" t="n">
         <v>-0.0062</v>
       </c>
       <c r="W52" t="n">
-        <v>-0.1052</v>
+        <v>-0.1176</v>
       </c>
     </row>
     <row r="53">
@@ -4241,31 +4241,31 @@
         <v>0.0137</v>
       </c>
       <c r="O53" t="n">
-        <v>0.0185</v>
+        <v>0.0251</v>
       </c>
       <c r="P53" t="n">
-        <v>0.0169</v>
+        <v>0.0277</v>
       </c>
       <c r="Q53" t="n">
-        <v>0.0194</v>
+        <v>0.0298</v>
       </c>
       <c r="R53" t="n">
-        <v>0.0216</v>
+        <v>0.0297</v>
       </c>
       <c r="S53" t="n">
-        <v>0.023</v>
+        <v>0.0296</v>
       </c>
       <c r="T53" t="n">
-        <v>0.0254</v>
+        <v>0.032</v>
       </c>
       <c r="U53" t="n">
-        <v>0.0274</v>
+        <v>0.0339</v>
       </c>
       <c r="V53" t="n">
-        <v>0.0423</v>
+        <v>0.0487</v>
       </c>
       <c r="W53" t="n">
-        <v>0.0886</v>
+        <v>0.092</v>
       </c>
     </row>
     <row r="54">
@@ -4312,13 +4312,13 @@
         <v>0.0005</v>
       </c>
       <c r="O54" t="n">
-        <v>0</v>
+        <v>0.0017</v>
       </c>
       <c r="P54" t="n">
-        <v>0</v>
+        <v>0.0016</v>
       </c>
       <c r="Q54" t="n">
-        <v>0</v>
+        <v>0.0007</v>
       </c>
       <c r="R54" t="n">
         <v>0</v>
@@ -4525,31 +4525,31 @@
         <v>-0.0003</v>
       </c>
       <c r="O57" t="n">
-        <v>0</v>
+        <v>-0.0058</v>
       </c>
       <c r="P57" t="n">
-        <v>-0.0001</v>
+        <v>-0.0063</v>
       </c>
       <c r="Q57" t="n">
-        <v>-0.0002</v>
+        <v>-0.0082</v>
       </c>
       <c r="R57" t="n">
-        <v>-0.0001</v>
+        <v>-0.0096</v>
       </c>
       <c r="S57" t="n">
-        <v>-0.0002</v>
+        <v>-0.0094</v>
       </c>
       <c r="T57" t="n">
-        <v>-0.0003</v>
+        <v>-0.0073</v>
       </c>
       <c r="U57" t="n">
-        <v>-0.0003</v>
+        <v>-0.0057</v>
       </c>
       <c r="V57" t="n">
-        <v>-0.0007</v>
+        <v>-0.0044</v>
       </c>
       <c r="W57" t="n">
-        <v>-0.0018</v>
+        <v>0.0094</v>
       </c>
     </row>
     <row r="58">

</xml_diff>